<commit_message>
Remove Provincia Certificado and Add Provincia Facturas
</commit_message>
<xml_diff>
--- a/templates/plantilla_certificado.xlsx
+++ b/templates/plantilla_certificado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25813"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AUTOMATIZACION NUEVO\crm-backend\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chapo\tumi_crm\crm-backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E86F26-649A-47DC-9169-580A7D0F19B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B926F19-5F3D-4C37-8817-5F03E86F5591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>EFICACIA</t>
-  </si>
-  <si>
-    <t>PROVINCIA</t>
   </si>
   <si>
     <t>FECHA FABRICACION</t>
@@ -187,9 +184,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,9 +224,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,9 +259,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -297,9 +311,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -473,27 +504,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -501,140 +531,136 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>